<commit_message>
Subida de código con cambios de Roberto Piqueras que no estaban en GIT
</commit_message>
<xml_diff>
--- a/GCS/war/datadocs/templateCartera.xlsx
+++ b/GCS/war/datadocs/templateCartera.xlsx
@@ -17,14 +17,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>SERVICIO</t>
   </si>
   <si>
-    <t>COD. SERVICIO</t>
-  </si>
-  <si>
     <t>FORMATO INTERMEDIO</t>
   </si>
   <si>
@@ -176,6 +173,12 @@
   </si>
   <si>
     <t xml:space="preserve">FECHA PASO ANS </t>
+  </si>
+  <si>
+    <t>COD. REDMINE</t>
+  </si>
+  <si>
+    <t>PETICIÓN</t>
   </si>
 </sst>
 </file>
@@ -540,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BA1"/>
+  <dimension ref="A1:BB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AJ21" sqref="AJ21"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -565,186 +568,189 @@
     <col min="15" max="15" width="20.7109375" customWidth="1"/>
     <col min="16" max="16" width="31.85546875" customWidth="1"/>
     <col min="17" max="19" width="28.42578125" customWidth="1"/>
-    <col min="20" max="20" width="20.85546875" customWidth="1"/>
-    <col min="21" max="21" width="18" customWidth="1"/>
-    <col min="22" max="22" width="24" customWidth="1"/>
-    <col min="23" max="23" width="22.28515625" customWidth="1"/>
-    <col min="24" max="25" width="30.140625" customWidth="1"/>
-    <col min="26" max="26" width="34.5703125" customWidth="1"/>
-    <col min="27" max="27" width="41" customWidth="1"/>
-    <col min="28" max="28" width="26.85546875" customWidth="1"/>
-    <col min="29" max="29" width="24.140625" customWidth="1"/>
-    <col min="30" max="30" width="26.5703125" customWidth="1"/>
-    <col min="31" max="31" width="23.85546875" customWidth="1"/>
-    <col min="32" max="32" width="46.140625" customWidth="1"/>
-    <col min="33" max="33" width="34.5703125" customWidth="1"/>
-    <col min="34" max="34" width="31.85546875" customWidth="1"/>
-    <col min="35" max="35" width="33.42578125" customWidth="1"/>
-    <col min="36" max="36" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="27.140625" customWidth="1"/>
-    <col min="38" max="38" width="30.5703125" customWidth="1"/>
-    <col min="39" max="53" width="33.85546875" customWidth="1"/>
+    <col min="20" max="21" width="20.85546875" customWidth="1"/>
+    <col min="22" max="22" width="18" customWidth="1"/>
+    <col min="23" max="23" width="24" customWidth="1"/>
+    <col min="24" max="24" width="22.28515625" customWidth="1"/>
+    <col min="25" max="26" width="30.140625" customWidth="1"/>
+    <col min="27" max="27" width="34.5703125" customWidth="1"/>
+    <col min="28" max="28" width="41" customWidth="1"/>
+    <col min="29" max="29" width="26.85546875" customWidth="1"/>
+    <col min="30" max="30" width="24.140625" customWidth="1"/>
+    <col min="31" max="31" width="26.5703125" customWidth="1"/>
+    <col min="32" max="32" width="23.85546875" customWidth="1"/>
+    <col min="33" max="33" width="46.140625" customWidth="1"/>
+    <col min="34" max="34" width="34.5703125" customWidth="1"/>
+    <col min="35" max="35" width="31.85546875" customWidth="1"/>
+    <col min="36" max="36" width="33.42578125" customWidth="1"/>
+    <col min="37" max="37" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="27.140625" customWidth="1"/>
+    <col min="39" max="39" width="30.5703125" customWidth="1"/>
+    <col min="40" max="54" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53">
+    <row r="1" spans="1:54">
       <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="X1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en excel Cartera para que aparezca el campo subtipo de producto
</commit_message>
<xml_diff>
--- a/GCS/war/datadocs/templateCartera.xlsx
+++ b/GCS/war/datadocs/templateCartera.xlsx
@@ -43,9 +43,6 @@
     <t xml:space="preserve">TIPO PROYECTO </t>
   </si>
   <si>
-    <t>CÓDIGO PROYECTO</t>
-  </si>
-  <si>
     <t xml:space="preserve">PRODUCTO </t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>PETICIÓN</t>
+  </si>
+  <si>
+    <t>SUBTIPO PRODUCTO</t>
   </si>
 </sst>
 </file>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -556,18 +556,18 @@
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
-    <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" customWidth="1"/>
-    <col min="11" max="11" width="24.5703125" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" customWidth="1"/>
-    <col min="13" max="13" width="22.85546875" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
-    <col min="16" max="16" width="31.85546875" customWidth="1"/>
-    <col min="17" max="19" width="28.42578125" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" customWidth="1"/>
+    <col min="7" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" customWidth="1"/>
+    <col min="12" max="12" width="24.5703125" customWidth="1"/>
+    <col min="13" max="13" width="25.5703125" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" customWidth="1"/>
+    <col min="15" max="15" width="32.140625" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
+    <col min="17" max="17" width="31.85546875" customWidth="1"/>
+    <col min="18" max="19" width="28.42578125" customWidth="1"/>
     <col min="20" max="21" width="20.85546875" customWidth="1"/>
     <col min="22" max="22" width="18" customWidth="1"/>
     <col min="23" max="23" width="24" customWidth="1"/>
@@ -606,55 +606,55 @@
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>1</v>
@@ -663,94 +663,94 @@
         <v>2</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en el informe cartera de posicion
</commit_message>
<xml_diff>
--- a/GCS/war/datadocs/templateCartera.xlsx
+++ b/GCS/war/datadocs/templateCartera.xlsx
@@ -70,9 +70,6 @@
     <t xml:space="preserve">FECHA ALTA PROYECTO </t>
   </si>
   <si>
-    <t xml:space="preserve">SUBTIPO PROYECTO </t>
-  </si>
-  <si>
     <t xml:space="preserve">CLASIFICACIÓN PROYECTO </t>
   </si>
   <si>
@@ -178,7 +175,10 @@
     <t>PETICIÓN</t>
   </si>
   <si>
-    <t>SUBTIPO PRODUCTO</t>
+    <t xml:space="preserve">PROYECTO </t>
+  </si>
+  <si>
+    <t>SUBTIPO PROYECTO</t>
   </si>
 </sst>
 </file>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -556,8 +556,9 @@
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" customWidth="1"/>
-    <col min="7" max="8" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
     <col min="11" max="11" width="27.28515625" customWidth="1"/>
@@ -606,13 +607,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>9</v>
@@ -630,7 +631,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>13</v>
@@ -645,16 +646,16 @@
         <v>16</v>
       </c>
       <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="W1" s="2" t="s">
         <v>1</v>
@@ -663,94 +664,94 @@
         <v>2</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambio que arregla problemas en pantalla servicio con la actualizacion del gestor de pruebas
</commit_message>
<xml_diff>
--- a/GCS/war/datadocs/templateCartera.xlsx
+++ b/GCS/war/datadocs/templateCartera.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>SERVICIO</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>SUBTIPO PROYECTO</t>
+  </si>
+  <si>
+    <t>GESTOR DE PRUEBAS</t>
   </si>
 </sst>
 </file>
@@ -543,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB1"/>
+  <dimension ref="A1:BC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -567,30 +570,30 @@
     <col min="14" max="14" width="22.85546875" customWidth="1"/>
     <col min="15" max="15" width="32.140625" customWidth="1"/>
     <col min="16" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="17" width="31.85546875" customWidth="1"/>
-    <col min="18" max="19" width="28.42578125" customWidth="1"/>
-    <col min="20" max="21" width="20.85546875" customWidth="1"/>
-    <col min="22" max="22" width="18" customWidth="1"/>
-    <col min="23" max="23" width="24" customWidth="1"/>
-    <col min="24" max="24" width="22.28515625" customWidth="1"/>
-    <col min="25" max="26" width="30.140625" customWidth="1"/>
-    <col min="27" max="27" width="34.5703125" customWidth="1"/>
-    <col min="28" max="28" width="41" customWidth="1"/>
-    <col min="29" max="29" width="26.85546875" customWidth="1"/>
-    <col min="30" max="30" width="24.140625" customWidth="1"/>
-    <col min="31" max="31" width="26.5703125" customWidth="1"/>
-    <col min="32" max="32" width="23.85546875" customWidth="1"/>
-    <col min="33" max="33" width="46.140625" customWidth="1"/>
-    <col min="34" max="34" width="34.5703125" customWidth="1"/>
-    <col min="35" max="35" width="31.85546875" customWidth="1"/>
-    <col min="36" max="36" width="33.42578125" customWidth="1"/>
-    <col min="37" max="37" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="27.140625" customWidth="1"/>
-    <col min="39" max="39" width="30.5703125" customWidth="1"/>
-    <col min="40" max="54" width="33.85546875" customWidth="1"/>
+    <col min="17" max="18" width="31.85546875" customWidth="1"/>
+    <col min="19" max="20" width="28.42578125" customWidth="1"/>
+    <col min="21" max="22" width="20.85546875" customWidth="1"/>
+    <col min="23" max="23" width="18" customWidth="1"/>
+    <col min="24" max="24" width="24" customWidth="1"/>
+    <col min="25" max="25" width="22.28515625" customWidth="1"/>
+    <col min="26" max="27" width="30.140625" customWidth="1"/>
+    <col min="28" max="28" width="34.5703125" customWidth="1"/>
+    <col min="29" max="29" width="41" customWidth="1"/>
+    <col min="30" max="30" width="26.85546875" customWidth="1"/>
+    <col min="31" max="31" width="24.140625" customWidth="1"/>
+    <col min="32" max="32" width="26.5703125" customWidth="1"/>
+    <col min="33" max="33" width="23.85546875" customWidth="1"/>
+    <col min="34" max="34" width="46.140625" customWidth="1"/>
+    <col min="35" max="35" width="34.5703125" customWidth="1"/>
+    <col min="36" max="36" width="31.85546875" customWidth="1"/>
+    <col min="37" max="37" width="33.42578125" customWidth="1"/>
+    <col min="38" max="38" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="27.140625" customWidth="1"/>
+    <col min="40" max="40" width="30.5703125" customWidth="1"/>
+    <col min="41" max="55" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:55">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -643,114 +646,117 @@
         <v>15</v>
       </c>
       <c r="R1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambio formato_intermedio por formato entrada/salida
Descripcion del cambio:

Cambiar nombre de la etiqueta "Formato intermedio" de la entidad
Servicio por "Formato de entrada/salida", y convertir el campo de texto
asociado en un combo metiendo valores del correo de Sara de 6/11 a las
12:57.  Habrá que añadir a la lista el valor "Antiguo" y deberá aparecer
este valor pre-cargado cuando el estado del servicio sea:  Excluido por
Negocio , Excluido por Timeout, Implementado con OK, Implementado sin
OK. 
Para el resto de estados, o añadimos un nuevo valor "Pendiente" que sea
el que aparezca por defecto o que aparezca el campo vacio. El resto de
estados son: PDTE Doc Alcance en GCS, C-100 en confección, PDTE
Valoración IT, PDTE Plan de Trabajo IT, PDTE Visto Bueno del CL del plan
de trabajo, En Desarrollo, En Test - Conectividad, En Test -
Integración, En Test - Aceptación, Parado por Negocio - Producto, Parado
por Negocio, Parado por IT, PDTE Implantar, En Penny Test
</commit_message>
<xml_diff>
--- a/GCS/war/datadocs/templateCartera.xlsx
+++ b/GCS/war/datadocs/templateCartera.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19440" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Cartera" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
     <t>SERVICIO</t>
   </si>
   <si>
-    <t>FORMATO INTERMEDIO</t>
-  </si>
-  <si>
     <t>FORMATO LOCAL</t>
   </si>
   <si>
@@ -182,6 +179,9 @@
   </si>
   <si>
     <t>GESTOR DE PRUEBAS</t>
+  </si>
+  <si>
+    <t>FORMATO ENTRADA/SALIDA</t>
   </si>
 </sst>
 </file>
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BC1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -574,7 +574,7 @@
     <col min="19" max="20" width="28.42578125" customWidth="1"/>
     <col min="21" max="22" width="20.85546875" customWidth="1"/>
     <col min="23" max="23" width="18" customWidth="1"/>
-    <col min="24" max="24" width="24" customWidth="1"/>
+    <col min="24" max="24" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="22.28515625" customWidth="1"/>
     <col min="26" max="27" width="30.140625" customWidth="1"/>
     <col min="28" max="28" width="34.5703125" customWidth="1"/>
@@ -595,169 +595,169 @@
   <sheetData>
     <row r="1" spans="1:55">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="W1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Meter en el formulario y entidad SERVICIO nuevos campos: - Tipo de Desarrollo (campo obligatorio): copiar valores de campo "Tipo desarrollo" de entidad Coste - Ocultar fechas salvo: fecha inicio integradas, fecha fin aceptación, Fecha Implantación-Producción, Fecha inicio primera operación, Fecha fin primera operación - Meter nuevo campo "Escenario OPI": 1/2/3 - Meter nuevo campo "Flujo": B-C/C-B
</commit_message>
<xml_diff>
--- a/GCS/war/datadocs/templateCartera.xlsx
+++ b/GCS/war/datadocs/templateCartera.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>SERVICIO</t>
   </si>
@@ -182,6 +182,15 @@
   </si>
   <si>
     <t>FORMATO ENTRADA/SALIDA</t>
+  </si>
+  <si>
+    <t>ESCENARIO OPI</t>
+  </si>
+  <si>
+    <t>FLUJO</t>
+  </si>
+  <si>
+    <t>TIPO DE DESARROLLO</t>
   </si>
 </sst>
 </file>
@@ -546,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC1"/>
+  <dimension ref="A1:BF1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -566,34 +575,34 @@
     <col min="10" max="10" width="16.5703125" customWidth="1"/>
     <col min="11" max="11" width="27.28515625" customWidth="1"/>
     <col min="12" max="12" width="24.5703125" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" customWidth="1"/>
-    <col min="15" max="15" width="32.140625" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1"/>
-    <col min="17" max="18" width="31.85546875" customWidth="1"/>
-    <col min="19" max="20" width="28.42578125" customWidth="1"/>
-    <col min="21" max="22" width="20.85546875" customWidth="1"/>
-    <col min="23" max="23" width="18" customWidth="1"/>
-    <col min="24" max="24" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.28515625" customWidth="1"/>
-    <col min="26" max="27" width="30.140625" customWidth="1"/>
-    <col min="28" max="28" width="34.5703125" customWidth="1"/>
-    <col min="29" max="29" width="41" customWidth="1"/>
-    <col min="30" max="30" width="26.85546875" customWidth="1"/>
-    <col min="31" max="31" width="24.140625" customWidth="1"/>
-    <col min="32" max="32" width="26.5703125" customWidth="1"/>
-    <col min="33" max="33" width="23.85546875" customWidth="1"/>
-    <col min="34" max="34" width="46.140625" customWidth="1"/>
-    <col min="35" max="35" width="34.5703125" customWidth="1"/>
-    <col min="36" max="36" width="31.85546875" customWidth="1"/>
-    <col min="37" max="37" width="33.42578125" customWidth="1"/>
-    <col min="38" max="38" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27.140625" customWidth="1"/>
-    <col min="40" max="40" width="30.5703125" customWidth="1"/>
-    <col min="41" max="55" width="33.85546875" customWidth="1"/>
+    <col min="13" max="16" width="25.5703125" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" customWidth="1"/>
+    <col min="18" max="18" width="32.140625" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="21" width="31.85546875" customWidth="1"/>
+    <col min="22" max="23" width="28.42578125" customWidth="1"/>
+    <col min="24" max="25" width="20.85546875" customWidth="1"/>
+    <col min="26" max="26" width="18" customWidth="1"/>
+    <col min="27" max="27" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.28515625" customWidth="1"/>
+    <col min="29" max="30" width="30.140625" customWidth="1"/>
+    <col min="31" max="31" width="34.5703125" customWidth="1"/>
+    <col min="32" max="32" width="41" customWidth="1"/>
+    <col min="33" max="33" width="26.85546875" customWidth="1"/>
+    <col min="34" max="34" width="24.140625" customWidth="1"/>
+    <col min="35" max="35" width="26.5703125" customWidth="1"/>
+    <col min="36" max="36" width="23.85546875" customWidth="1"/>
+    <col min="37" max="37" width="46.140625" customWidth="1"/>
+    <col min="38" max="38" width="34.5703125" customWidth="1"/>
+    <col min="39" max="39" width="31.85546875" customWidth="1"/>
+    <col min="40" max="40" width="33.42578125" customWidth="1"/>
+    <col min="41" max="41" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="27.140625" customWidth="1"/>
+    <col min="43" max="43" width="30.5703125" customWidth="1"/>
+    <col min="44" max="58" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55">
+    <row r="1" spans="1:58">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -634,129 +643,138 @@
         <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>